<commit_message>
GenLouvain community detection. some changes in aggregate_CAMs and data preparation were necessary.
</commit_message>
<xml_diff>
--- a/partII_CAMs/outputs/01_dataPreperation/final/CAMwordlist.xlsx
+++ b/partII_CAMs/outputs/01_dataPreperation/final/CAMwordlist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="332">
   <si>
     <t>Words</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>comment_19</t>
+  </si>
+  <si>
+    <t>mean_transitivity</t>
+  </si>
+  <si>
+    <t>sd_transitivity</t>
   </si>
   <si>
     <t>1</t>
@@ -1160,13 +1166,19 @@
       <c r="AA1" t="s">
         <v>25</v>
       </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C2" t="n">
         <v>186.0</v>
@@ -1187,69 +1199,75 @@
         <v>8.819401151744096</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="M2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA2" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.05689396431337302</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.11376179957922743</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" t="n">
         <v>186.0</v>
@@ -1270,69 +1288,75 @@
         <v>1.9055891424063782</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="L3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="N3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA3" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.36794537363817703</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>0.3896714219499534</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" t="n">
         <v>186.0</v>
@@ -1353,69 +1377,75 @@
         <v>1.0945560248800783</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="L4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA4" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.48032128514056227</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>0.42301781163298774</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C5" t="n">
         <v>186.0</v>
@@ -1436,69 +1466,75 @@
         <v>1.1225541723254557</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="J5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K5" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="L5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="N5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="O5" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="P5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Q5" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="R5" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="S5" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="T5" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="U5" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="V5" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="W5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA5" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.44828869047619047</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.461540222225728</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C6" t="n">
         <v>186.0</v>
@@ -1519,69 +1555,75 @@
         <v>0.965790922998169</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="L6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="M6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="O6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="P6" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="Q6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="R6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z6" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA6" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.34202898550724636</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.42716775775464627</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7" t="n">
         <v>186.0</v>
@@ -1602,69 +1644,75 @@
         <v>0.8520450806906913</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="M7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="N7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="O7" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="P7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA7" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.38606965174129354</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.45342502243191796</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C8" t="n">
         <v>186.0</v>
@@ -1685,69 +1733,75 @@
         <v>1.677318475494734</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="L8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M8" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="N8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="O8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="P8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA8" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.23532743851892787</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.3683923374898022</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C9" t="n">
         <v>186.0</v>
@@ -1768,69 +1822,75 @@
         <v>1.6302145671717236</v>
       </c>
       <c r="I9" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K9" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="L9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA9" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.24996488270824552</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.35955910393658086</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C10" t="n">
         <v>186.0</v>
@@ -1851,69 +1911,75 @@
         <v>1.0808630992095072</v>
       </c>
       <c r="I10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K10" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="M10" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="N10" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="O10" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="P10" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="Q10" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="R10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA10" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.35035014005602244</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.4175583442395314</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
         <v>186.0</v>
@@ -1934,69 +2000,75 @@
         <v>1.273018230083058</v>
       </c>
       <c r="I11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K11" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="M11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z11" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA11" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.3036231884057971</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.3971958031316237</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" t="n">
         <v>186.0</v>
@@ -2017,69 +2089,75 @@
         <v>1.5377455692113626</v>
       </c>
       <c r="I12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K12" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z12" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA12" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.3371087375760273</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.40633481417078166</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C13" t="n">
         <v>186.0</v>
@@ -2100,69 +2178,75 @@
         <v>1.1811387035501466</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J13" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K13" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="L13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M13" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="N13" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="O13" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="P13" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="Q13" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="R13" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="S13" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="T13" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="U13" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="V13" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="W13" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="X13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="Y13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="Z13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AA13" t="s">
-        <v>329</v>
+        <v>331</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.40534722222222225</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.4412769014557637</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C14" t="n">
         <v>186.0</v>
@@ -2183,69 +2267,75 @@
         <v>2.001539657291203</v>
       </c>
       <c r="I14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="J14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="L14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="M14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA14" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.37331349206349207</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.3910193603746583</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C15" t="n">
         <v>186.0</v>
@@ -2266,69 +2356,75 @@
         <v>2.477618500120997</v>
       </c>
       <c r="I15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="L15" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M15" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="N15" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="O15" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="P15" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="Q15" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="R15" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="S15" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="T15" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="U15" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="V15" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="W15" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="X15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z15" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA15" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0.21734052111410598</v>
+      </c>
+      <c r="AC15" t="n">
+        <v>0.32215198666431</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" t="n">
         <v>186.0</v>
@@ -2349,69 +2445,75 @@
         <v>2.399826836725021</v>
       </c>
       <c r="I16" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="L16" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="M16" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="N16" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="O16" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="P16" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="Q16" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="R16" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="S16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z16" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA16" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.34193986928104575</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0.3639908132010843</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C17" t="n">
         <v>186.0</v>
@@ -2432,69 +2534,75 @@
         <v>1.6709216246880174</v>
       </c>
       <c r="I17" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K17" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L17" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M17" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="N17" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="O17" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="P17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z17" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA17" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0.24537318473488684</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0.3310940322401557</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C18" t="n">
         <v>186.0</v>
@@ -2515,69 +2623,75 @@
         <v>1.1165188562186381</v>
       </c>
       <c r="I18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K18" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L18" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M18" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="N18" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="O18" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="P18" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="Q18" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="R18" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="S18" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="T18" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="U18" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="V18" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="W18" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="X18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z18" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA18" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0.4094062316284538</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>0.42330559614300817</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C19" t="n">
         <v>186.0</v>
@@ -2598,69 +2712,75 @@
         <v>1.5454369842366398</v>
       </c>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K19" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="L19" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M19" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="N19" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="O19" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="P19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z19" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA19" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0.27559523809523806</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0.3933194950170748</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C20" t="n">
         <v>186.0</v>
@@ -2681,69 +2801,75 @@
         <v>2.7536296091543444</v>
       </c>
       <c r="I20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="K20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="L20" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M20" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="N20" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="O20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z20" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA20" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0.2203220015004912</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0.3017504751563466</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C21" t="n">
         <v>186.0</v>
@@ -2764,69 +2890,75 @@
         <v>0.9038166996476918</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="K21" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="L21" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M21" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="N21" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="O21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA21" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.41690821256038646</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0.4494958391631963</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C22" t="n">
         <v>186.0</v>
@@ -2847,69 +2979,75 @@
         <v>0.8587041730000475</v>
       </c>
       <c r="I22" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J22" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="K22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="L22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="M22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z22" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA22" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>0.35654761904761906</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>0.4316713884312784</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23" t="n">
         <v>186.0</v>
@@ -2930,69 +3068,75 @@
         <v>1.4437933986854785</v>
       </c>
       <c r="I23" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K23" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="L23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="M23" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="N23" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="O23" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="P23" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="Q23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA23" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>0.3044248749728202</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>0.41298016256242365</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C24" t="n">
         <v>186.0</v>
@@ -3013,69 +3157,75 @@
         <v>1.7310354070193215</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="M24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z24" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA24" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB24" t="n">
+        <v>0.37918706423379317</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.3806844499983209</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C25" t="n">
         <v>186.0</v>
@@ -3096,69 +3246,75 @@
         <v>1.5861669530734706</v>
       </c>
       <c r="I25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K25" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="L25" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="M25" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N25" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="O25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z25" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA25" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>0.36614583333333334</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>0.40751874281711076</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C26" t="n">
         <v>186.0</v>
@@ -3179,69 +3335,75 @@
         <v>1.4115910751903702</v>
       </c>
       <c r="I26" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J26" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K26" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="L26" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M26" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="N26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z26" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA26" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB26" t="n">
+        <v>0.43056668150126093</v>
+      </c>
+      <c r="AC26" t="n">
+        <v>0.41648583997433053</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C27" t="n">
         <v>186.0</v>
@@ -3262,69 +3424,75 @@
         <v>3.376453156759436</v>
       </c>
       <c r="I27" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J27" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K27" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L27" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="M27" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="N27" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="O27" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="P27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z27" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA27" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>0.24793522682475008</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0.3440469473938018</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C28" t="n">
         <v>186.0</v>
@@ -3345,69 +3513,75 @@
         <v>2.23311579659446</v>
       </c>
       <c r="I28" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J28" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K28" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L28" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M28" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="N28" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="O28" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="P28" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="Q28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z28" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA28" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>0.23640444522797463</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.30460522732632617</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C29" t="n">
         <v>186.0</v>
@@ -3428,69 +3602,75 @@
         <v>1.3579391877205786</v>
       </c>
       <c r="I29" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J29" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K29" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L29" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M29" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="N29" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="O29" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="P29" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="Q29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z29" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA29" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>0.28593576965669987</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.3677085973313867</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C30" t="n">
         <v>186.0</v>
@@ -3511,69 +3691,75 @@
         <v>1.6227100870877749</v>
       </c>
       <c r="I30" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J30" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="L30" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="M30" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="N30" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="O30" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="P30" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="Q30" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="R30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z30" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA30" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>0.35534373882997733</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.391412096267067</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C31" t="n">
         <v>186.0</v>
@@ -3594,69 +3780,75 @@
         <v>1.1715036525357823</v>
       </c>
       <c r="I31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J31" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="K31" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="L31" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="M31" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="N31" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="O31" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="P31" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="Q31" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="R31" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="S31" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="T31" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="U31" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="V31" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="W31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z31" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA31" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.4497777777777778</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.43929965192813913</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C32" t="n">
         <v>186.0</v>
@@ -3677,69 +3869,75 @@
         <v>1.5567628616400042</v>
       </c>
       <c r="I32" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J32" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K32" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L32" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="M32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="N32" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="O32" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="P32" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="Q32" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="R32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA32" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.3973356009070295</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.4081702210747002</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C33" t="n">
         <v>186.0</v>
@@ -3760,69 +3958,75 @@
         <v>1.6391834571753232</v>
       </c>
       <c r="I33" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J33" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K33" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="L33" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="M33" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="N33" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="O33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z33" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA33" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.3553375196232339</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.4022070537253573</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C34" t="n">
         <v>186.0</v>
@@ -3843,61 +4047,67 @@
         <v>2.3865176375162434</v>
       </c>
       <c r="I34" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J34" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K34" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="L34" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="M34" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="N34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="O34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="P34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="R34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="T34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="U34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="V34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="W34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="X34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Y34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Z34" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AA34" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0.37448634444047285</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.4096735762357971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>